<commit_message>
29/03 done Unit Test
</commit_message>
<xml_diff>
--- a/MAR-2024/2103/UT/Practice_UT.xlsx
+++ b/MAR-2024/2103/UT/Practice_UT.xlsx
@@ -8,24 +8,40 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\long.trinh-tien\Documents\Linux-Lab\MAR-2024\2103\UT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA2F99B2-6704-444A-B0E0-C1200711B3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3A8826-BFCD-4A2D-8062-96EF358E0461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Revision" sheetId="5" r:id="rId1"/>
     <sheet name="Practice_Unit_Testing" sheetId="6" r:id="rId2"/>
     <sheet name="template" sheetId="8" r:id="rId3"/>
-    <sheet name="data_format_convert" sheetId="9" r:id="rId4"/>
-    <sheet name="DMA_API" sheetId="10" r:id="rId5"/>
+    <sheet name="DMA_API" sheetId="10" r:id="rId4"/>
+    <sheet name="data_format_convert" sheetId="9" r:id="rId5"/>
     <sheet name="pre_check_config" sheetId="11" r:id="rId6"/>
+    <sheet name="MCDC check_noise" sheetId="12" r:id="rId7"/>
+    <sheet name="check_noise" sheetId="13" r:id="rId8"/>
+    <sheet name="crop_image_and_divide" sheetId="14" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="199">
   <si>
     <t>Version</t>
   </si>
@@ -924,6 +940,291 @@
   </si>
   <si>
     <t>square_shift</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Check for independent A</t>
+  </si>
+  <si>
+    <t>Check for A</t>
+  </si>
+  <si>
+    <t>x15</t>
+  </si>
+  <si>
+    <t>x8</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>x11</t>
+  </si>
+  <si>
+    <t>x4</t>
+  </si>
+  <si>
+    <t>x13</t>
+  </si>
+  <si>
+    <t>x6</t>
+  </si>
+  <si>
+    <t>x14</t>
+  </si>
+  <si>
+    <t>x9</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>Num</t>
+  </si>
+  <si>
+    <t>x10</t>
+  </si>
+  <si>
+    <t>(4,11)</t>
+  </si>
+  <si>
+    <t>x12</t>
+  </si>
+  <si>
+    <t>x16</t>
+  </si>
+  <si>
+    <t>x5</t>
+  </si>
+  <si>
+    <t>x7</t>
+  </si>
+  <si>
+    <t>Check for B</t>
+  </si>
+  <si>
+    <t>(4,7)</t>
+  </si>
+  <si>
+    <t>Check for independent B</t>
+  </si>
+  <si>
+    <t>Check for C</t>
+  </si>
+  <si>
+    <t>Check for D</t>
+  </si>
+  <si>
+    <t>(3,4)</t>
+  </si>
+  <si>
+    <t>(7,8)</t>
+  </si>
+  <si>
+    <t>(2,9)</t>
+  </si>
+  <si>
+    <t>(1,15)</t>
+  </si>
+  <si>
+    <t>(3,5)</t>
+  </si>
+  <si>
+    <t>(10,12)</t>
+  </si>
+  <si>
+    <t>(11,16)</t>
+  </si>
+  <si>
+    <t>(13,14)</t>
+  </si>
+  <si>
+    <t>Check for independent C</t>
+  </si>
+  <si>
+    <t>Check for independent D (at least 1, so I choose 1 )</t>
+  </si>
+  <si>
+    <t>In total, all case we need to test are</t>
+  </si>
+  <si>
+    <t>N+1 (N is number of condition)</t>
+  </si>
+  <si>
+    <t>p_noise</t>
+  </si>
+  <si>
+    <t>check_noise_0001</t>
+  </si>
+  <si>
+    <t>Stub is_DMA_Check returns E_FAILURE</t>
+  </si>
+  <si>
+    <t>check_noise_0002</t>
+  </si>
+  <si>
+    <t>Stubis_DMA_Check  returns E_SUCCESS</t>
+  </si>
+  <si>
+    <t>check_noise_0003</t>
+  </si>
+  <si>
+    <t>Stub is_DMA_Check  returns E_FAILURE</t>
+  </si>
+  <si>
+    <t>check_noise_0004</t>
+  </si>
+  <si>
+    <t>Stub is_DMA_Check  returns E_SUCCESS</t>
+  </si>
+  <si>
+    <t>&gt;10</t>
+  </si>
+  <si>
+    <t>&gt;11</t>
+  </si>
+  <si>
+    <t>&gt;12</t>
+  </si>
+  <si>
+    <t>&gt;9</t>
+  </si>
+  <si>
+    <t>check_noise_0005</t>
+  </si>
+  <si>
+    <t>check_noise_0006</t>
+  </si>
+  <si>
+    <t>*p_image_config</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>divisor</t>
+  </si>
+  <si>
+    <t>crop_image_and_divide_0001</t>
+  </si>
+  <si>
+    <t>Check NULL p_dma_config</t>
+  </si>
+  <si>
+    <t>crop_image_and_divide_0002</t>
+  </si>
+  <si>
+    <t>Normal operation</t>
+  </si>
+  <si>
+    <t>crop_image_and_divide_0003</t>
+  </si>
+  <si>
+    <t>crop_image_and_divide_0004</t>
+  </si>
+  <si>
+    <t>crop_image_and_divide_0005</t>
+  </si>
+  <si>
+    <t>crop_image_and_divide_0006</t>
+  </si>
+  <si>
+    <t>crop_image_and_divide_0007</t>
+  </si>
+  <si>
+    <t>crop_image_and_divide_0008</t>
+  </si>
+  <si>
+    <t>p_image == NULL</t>
+  </si>
+  <si>
+    <t>width_of_image &lt;= 500</t>
+  </si>
+  <si>
+    <t>height_of_image &lt;= 500</t>
+  </si>
+  <si>
+    <t>width_of_image % 2 != 0</t>
+  </si>
+  <si>
+    <t>width_of_image % 5 != 0</t>
+  </si>
+  <si>
+    <t>width_of_image % 6 != 0</t>
+  </si>
+  <si>
+    <t>divisor % 60 == 0</t>
+  </si>
+  <si>
+    <t>divisor % 120 == 0</t>
+  </si>
+  <si>
+    <t>divisor % 180 == 0</t>
+  </si>
+  <si>
+    <t>divisor &lt;= width_of_image</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>số chẳn ko chia hết cho 6</t>
+  </si>
+  <si>
+    <t>số lẻ đuôi là 5</t>
+  </si>
+  <si>
+    <t>số lẻ ko chia hết cho 5 và 6</t>
+  </si>
+  <si>
+    <t>số lẻ ko chia hết cho 5 nhưng chia hết cho 6</t>
+  </si>
+  <si>
+    <t>MCDC</t>
+  </si>
+  <si>
+    <t>ko thể kiểm tra tính độc lập của %120 và %180 -&gt; chuyển lên T để coverage C2</t>
+  </si>
+  <si>
+    <t>width_of_image = height_of_image</t>
+  </si>
+  <si>
+    <t>Ko thể kiểm tra tính độc lập của %6, chuyển qua F để check coverage C2</t>
+  </si>
+  <si>
+    <t>Chỉ có 1 trường hợp result true duy nhất-&gt;chỉ có thể kiểm tra tính độc lập dựa trên case này</t>
+  </si>
+  <si>
+    <t>Chỉ có 1 trường hợp result False duy nhất-&gt;chỉ có thể kiểm tra tính độc lập dựa trên case này</t>
+  </si>
+  <si>
+    <t>divisor được chọn</t>
   </si>
 </sst>
 </file>
@@ -1120,7 +1421,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1192,8 +1493,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1330,6 +1649,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1352,7 +1702,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1538,6 +1888,38 @@
     <xf numFmtId="0" fontId="11" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Bad 2" xfId="7" xr:uid="{16D7B6FD-A74C-4A12-A91D-77110C66813E}"/>
@@ -1551,7 +1933,638 @@
     <cellStyle name="標準 2 2 2" xfId="9" xr:uid="{EAFC57A7-1694-4442-A10B-F0AB8BF706EF}"/>
     <cellStyle name="標準 4 3" xfId="6" xr:uid="{1F65E3D5-2742-4271-ACFD-934ED4073383}"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="63">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
@@ -1957,8 +2970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A85911D-DE00-4BEB-A94B-8AC5959916A5}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2048,7 +3061,9 @@
       <c r="D5" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="39"/>
+      <c r="E5" s="39" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="207.9" customHeight="1">
       <c r="A6" s="17">
@@ -2063,7 +3078,9 @@
       <c r="D6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="39"/>
+      <c r="E6" s="39" t="s">
+        <v>82</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2947,412 +3964,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845C65B1-29D9-4132-B49A-B9F56DDB7321}">
-  <dimension ref="A1:K21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="6.54296875" customWidth="1"/>
-    <col min="2" max="2" width="35.54296875" customWidth="1"/>
-    <col min="3" max="3" width="38.453125" customWidth="1"/>
-    <col min="4" max="4" width="25.1796875" customWidth="1"/>
-    <col min="5" max="5" width="23.90625" customWidth="1"/>
-    <col min="6" max="6" width="30.1796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="49"/>
-      <c r="F1" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="58" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="58" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="26">
-        <v>1</v>
-      </c>
-      <c r="B4" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="27">
-        <v>5</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="27">
-        <v>-1</v>
-      </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="26">
-        <v>2</v>
-      </c>
-      <c r="B5" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" s="27">
-        <v>4</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="F5" s="27">
-        <v>0</v>
-      </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="26">
-        <v>3</v>
-      </c>
-      <c r="B6" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6" s="27">
-        <v>0</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="F6" s="27">
-        <v>10.25</v>
-      </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="26">
-        <v>4</v>
-      </c>
-      <c r="B7" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="D7" s="27">
-        <v>1</v>
-      </c>
-      <c r="E7" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7" s="27">
-        <v>9.75</v>
-      </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="26">
-        <v>5</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8" s="27">
-        <v>2</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="F8" s="27">
-        <v>8.5</v>
-      </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="26">
-        <v>6</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="D9" s="27">
-        <v>3</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="F9" s="27">
-        <v>7.75</v>
-      </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="26">
-        <v>7</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="D10" s="27">
-        <v>4</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="F10" s="27">
-        <v>0</v>
-      </c>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="23"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="23"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="23"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="23"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="23"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-    </row>
-  </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-  </mergeCells>
-  <phoneticPr fontId="10" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3A63687-D40C-43F5-B271-33AD5E9B3485}">
   <dimension ref="A1:V24"/>
   <sheetViews>
@@ -4376,12 +4987,418 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845C65B1-29D9-4132-B49A-B9F56DDB7321}">
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="6.54296875" customWidth="1"/>
+    <col min="2" max="2" width="35.54296875" customWidth="1"/>
+    <col min="3" max="3" width="38.453125" customWidth="1"/>
+    <col min="4" max="4" width="25.1796875" customWidth="1"/>
+    <col min="5" max="5" width="23.90625" customWidth="1"/>
+    <col min="6" max="6" width="30.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="49"/>
+      <c r="F1" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="58" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="26">
+        <v>1</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="27">
+        <v>5</v>
+      </c>
+      <c r="E4" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="27">
+        <v>-1</v>
+      </c>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="26">
+        <v>2</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="27">
+        <v>4</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="27">
+        <v>0</v>
+      </c>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="26">
+        <v>3</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="27">
+        <v>0</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="27">
+        <v>10.25</v>
+      </c>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="26">
+        <v>4</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="27">
+        <v>1</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="F7" s="27">
+        <v>9.75</v>
+      </c>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="26">
+        <v>5</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="27">
+        <v>2</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="F8" s="27">
+        <v>8.5</v>
+      </c>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="26">
+        <v>6</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="27">
+        <v>3</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="27">
+        <v>7.75</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="26">
+        <v>7</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="27">
+        <v>4</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="27">
+        <v>0</v>
+      </c>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+  </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEA4EF1B-FA69-444D-90F4-5E17BA603AD4}">
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5000,4 +6017,2519 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F9FD00-F68A-4765-A672-35EDD6F2B3DA}">
+  <dimension ref="A1:J36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="7" max="7" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="10.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" t="s">
+        <v>130</v>
+      </c>
+      <c r="J3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F4" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" t="s">
+        <v>125</v>
+      </c>
+      <c r="H4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I4" t="s">
+        <v>136</v>
+      </c>
+      <c r="J4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I5" t="s">
+        <v>136</v>
+      </c>
+      <c r="J5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H6" t="s">
+        <v>122</v>
+      </c>
+      <c r="I6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H7" t="s">
+        <v>114</v>
+      </c>
+      <c r="I7" t="s">
+        <v>82</v>
+      </c>
+      <c r="J7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F8" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" t="s">
+        <v>119</v>
+      </c>
+      <c r="H8" t="s">
+        <v>132</v>
+      </c>
+      <c r="I8" t="s">
+        <v>115</v>
+      </c>
+      <c r="J8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" t="s">
+        <v>120</v>
+      </c>
+      <c r="I9" t="s">
+        <v>82</v>
+      </c>
+      <c r="J9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E10" t="s">
+        <v>110</v>
+      </c>
+      <c r="F10" t="s">
+        <v>110</v>
+      </c>
+      <c r="G10" t="s">
+        <v>113</v>
+      </c>
+      <c r="H10" t="s">
+        <v>129</v>
+      </c>
+      <c r="I10" t="s">
+        <v>82</v>
+      </c>
+      <c r="J10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" t="s">
+        <v>109</v>
+      </c>
+      <c r="G11" t="s">
+        <v>123</v>
+      </c>
+      <c r="H11" t="s">
+        <v>116</v>
+      </c>
+      <c r="I11" t="s">
+        <v>82</v>
+      </c>
+      <c r="J11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" t="s">
+        <v>110</v>
+      </c>
+      <c r="E12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" t="s">
+        <v>126</v>
+      </c>
+      <c r="H12" t="s">
+        <v>119</v>
+      </c>
+      <c r="I12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" t="s">
+        <v>110</v>
+      </c>
+      <c r="F13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G13" t="s">
+        <v>129</v>
+      </c>
+      <c r="H13" t="s">
+        <v>113</v>
+      </c>
+      <c r="I13" t="s">
+        <v>82</v>
+      </c>
+      <c r="J13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" t="s">
+        <v>109</v>
+      </c>
+      <c r="F14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" t="s">
+        <v>130</v>
+      </c>
+      <c r="H14" t="s">
+        <v>117</v>
+      </c>
+      <c r="I14" t="s">
+        <v>116</v>
+      </c>
+      <c r="J14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D15" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" t="s">
+        <v>110</v>
+      </c>
+      <c r="F15" t="s">
+        <v>110</v>
+      </c>
+      <c r="G15" t="s">
+        <v>114</v>
+      </c>
+      <c r="H15" t="s">
+        <v>128</v>
+      </c>
+      <c r="I15" t="s">
+        <v>82</v>
+      </c>
+      <c r="J15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" t="s">
+        <v>109</v>
+      </c>
+      <c r="E16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" t="s">
+        <v>122</v>
+      </c>
+      <c r="H16" t="s">
+        <v>127</v>
+      </c>
+      <c r="I16" t="s">
+        <v>82</v>
+      </c>
+      <c r="J16" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" t="s">
+        <v>120</v>
+      </c>
+      <c r="H17" t="s">
+        <v>121</v>
+      </c>
+      <c r="I17" t="s">
+        <v>82</v>
+      </c>
+      <c r="J17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E20" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" t="s">
+        <v>109</v>
+      </c>
+      <c r="G20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" t="s">
+        <v>110</v>
+      </c>
+      <c r="G22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" t="s">
+        <v>110</v>
+      </c>
+      <c r="G25" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>110</v>
+      </c>
+      <c r="C26" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" t="s">
+        <v>109</v>
+      </c>
+      <c r="E26" t="s">
+        <v>109</v>
+      </c>
+      <c r="F26" t="s">
+        <v>109</v>
+      </c>
+      <c r="G26" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" t="s">
+        <v>109</v>
+      </c>
+      <c r="F28" t="s">
+        <v>109</v>
+      </c>
+      <c r="G28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" t="s">
+        <v>109</v>
+      </c>
+      <c r="E29" t="s">
+        <v>110</v>
+      </c>
+      <c r="F29" t="s">
+        <v>110</v>
+      </c>
+      <c r="G29" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
+        <v>146</v>
+      </c>
+      <c r="E31" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" t="s">
+        <v>109</v>
+      </c>
+      <c r="E32" t="s">
+        <v>109</v>
+      </c>
+      <c r="F32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" t="s">
+        <v>109</v>
+      </c>
+      <c r="F33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" t="s">
+        <v>109</v>
+      </c>
+      <c r="E34" t="s">
+        <v>110</v>
+      </c>
+      <c r="F34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35">
+        <v>7</v>
+      </c>
+      <c r="B35" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" t="s">
+        <v>110</v>
+      </c>
+      <c r="E35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F35" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36">
+        <v>11</v>
+      </c>
+      <c r="B36" t="s">
+        <v>109</v>
+      </c>
+      <c r="C36" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" t="s">
+        <v>110</v>
+      </c>
+      <c r="E36" t="s">
+        <v>109</v>
+      </c>
+      <c r="F36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A17:A18 B1:F17">
+    <cfRule type="cellIs" dxfId="62" priority="37" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="38" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19:F19">
+    <cfRule type="cellIs" dxfId="60" priority="35" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="36" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20:F20">
+    <cfRule type="cellIs" dxfId="58" priority="33" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="34" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:J1048576">
+    <cfRule type="containsText" dxfId="56" priority="29" operator="containsText" text="(*)">
+      <formula>NOT(ISERROR(SEARCH("(*)",G1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="cellIs" dxfId="55" priority="27" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="28" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22:F22">
+    <cfRule type="cellIs" dxfId="53" priority="25" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="26" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23:F23">
+    <cfRule type="cellIs" dxfId="51" priority="23" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="24" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24">
+    <cfRule type="cellIs" dxfId="49" priority="21" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="22" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25:F25">
+    <cfRule type="cellIs" dxfId="47" priority="19" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="20" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26:F26">
+    <cfRule type="cellIs" dxfId="45" priority="17" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="18" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28:F28">
+    <cfRule type="cellIs" dxfId="43" priority="15" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="16" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29:F29">
+    <cfRule type="cellIs" dxfId="41" priority="13" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="14" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27">
+    <cfRule type="cellIs" dxfId="39" priority="11" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="12" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32:F32">
+    <cfRule type="cellIs" dxfId="37" priority="9" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="10" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33:F33">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="8" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34:F34">
+    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35:F35">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="4" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B36:F36">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6633ED31-29EF-4F82-A738-78212703ADFF}">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="3.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="25.6328125" customWidth="1"/>
+    <col min="8" max="8" width="33.453125" customWidth="1"/>
+    <col min="9" max="9" width="21.26953125" customWidth="1"/>
+    <col min="10" max="10" width="33.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="65" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" s="66"/>
+      <c r="J2" s="55" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="55"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="26">
+        <v>1</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="71">
+        <v>0</v>
+      </c>
+      <c r="E4" s="71">
+        <v>0</v>
+      </c>
+      <c r="F4" s="71">
+        <v>0</v>
+      </c>
+      <c r="G4" s="71">
+        <v>0</v>
+      </c>
+      <c r="H4" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="26">
+        <v>2</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" s="71">
+        <v>11</v>
+      </c>
+      <c r="E5" s="71">
+        <v>12</v>
+      </c>
+      <c r="F5" s="71">
+        <v>12</v>
+      </c>
+      <c r="G5" s="71">
+        <v>9</v>
+      </c>
+      <c r="H5" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="26">
+        <v>3</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="71">
+        <v>11</v>
+      </c>
+      <c r="E6" s="71">
+        <v>12</v>
+      </c>
+      <c r="F6" s="71">
+        <v>13</v>
+      </c>
+      <c r="G6" s="71">
+        <v>9</v>
+      </c>
+      <c r="H6" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="26">
+        <v>4</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="71">
+        <v>11</v>
+      </c>
+      <c r="E7" s="71">
+        <v>12</v>
+      </c>
+      <c r="F7" s="71">
+        <v>12</v>
+      </c>
+      <c r="G7" s="71">
+        <v>10</v>
+      </c>
+      <c r="H7" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="27" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="26">
+        <v>5</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="71">
+        <v>11</v>
+      </c>
+      <c r="E8" s="71">
+        <v>11</v>
+      </c>
+      <c r="F8" s="71">
+        <v>13</v>
+      </c>
+      <c r="G8" s="71">
+        <v>9</v>
+      </c>
+      <c r="H8" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" s="30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="26">
+        <v>6</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="D9" s="71">
+        <v>10</v>
+      </c>
+      <c r="E9" s="71">
+        <v>12</v>
+      </c>
+      <c r="F9" s="71">
+        <v>13</v>
+      </c>
+      <c r="G9" s="71">
+        <v>9</v>
+      </c>
+      <c r="H9" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="D12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E12" t="s">
+        <v>158</v>
+      </c>
+      <c r="F12" t="s">
+        <v>159</v>
+      </c>
+      <c r="G12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="C13" s="26" t="s">
+        <v>151</v>
+      </c>
+      <c r="D13" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="F13" s="72" t="s">
+        <v>109</v>
+      </c>
+      <c r="G13" s="72" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="C14" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="D14" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="G14" s="72" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="C15" s="26" t="s">
+        <v>155</v>
+      </c>
+      <c r="D15" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="F15" s="72" t="s">
+        <v>109</v>
+      </c>
+      <c r="G15" s="72" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="C16" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="D16" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" s="72" t="s">
+        <v>109</v>
+      </c>
+      <c r="F16" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" s="72" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7">
+      <c r="C17" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="D17" s="72" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" s="72" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" s="72" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="H2:I3"/>
+    <mergeCell ref="D2:G3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D13:J13">
+    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14:J14">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15:J15">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:J16">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17:J17">
+    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D9">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="lessThanOrEqual">
+      <formula>10</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="greaterThan">
+      <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E9">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="lessThanOrEqual">
+      <formula>11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="17" operator="greaterThan">
+      <formula>11</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:F9">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="lessThanOrEqual">
+      <formula>12</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="greaterThan">
+      <formula>12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:G9">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="greaterThan">
+      <formula>9</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="lessThanOrEqual">
+      <formula>9</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K8">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"T"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC293A4C-C140-4849-9171-7DCA0DD68DBB}">
+  <dimension ref="A1:M44"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.54296875" customWidth="1"/>
+    <col min="3" max="3" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="73" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="45"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="I3" s="55"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="L3" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="26">
+        <v>1</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="29">
+        <v>0</v>
+      </c>
+      <c r="F4" s="29">
+        <v>0</v>
+      </c>
+      <c r="G4" s="29">
+        <v>0</v>
+      </c>
+      <c r="H4" s="29">
+        <v>0</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="29">
+        <f>L4</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="29">
+        <v>0</v>
+      </c>
+      <c r="M4" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="26">
+        <v>2</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="29">
+        <v>1</v>
+      </c>
+      <c r="F5" s="29">
+        <v>501</v>
+      </c>
+      <c r="G5" s="29">
+        <v>0</v>
+      </c>
+      <c r="H5" s="29">
+        <v>0</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" s="29">
+        <v>1</v>
+      </c>
+      <c r="L5" s="29">
+        <v>501</v>
+      </c>
+      <c r="M5" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="26">
+        <v>3</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="29">
+        <v>501</v>
+      </c>
+      <c r="F6" s="29">
+        <v>501</v>
+      </c>
+      <c r="G6" s="29">
+        <v>0</v>
+      </c>
+      <c r="H6" s="29">
+        <v>0</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="29">
+        <f t="shared" ref="K5:K11" si="0">L6</f>
+        <v>501</v>
+      </c>
+      <c r="L6" s="29">
+        <v>501</v>
+      </c>
+      <c r="M6" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="26">
+        <v>4</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="29">
+        <v>501</v>
+      </c>
+      <c r="F7" s="29">
+        <v>502</v>
+      </c>
+      <c r="G7" s="29">
+        <v>0</v>
+      </c>
+      <c r="H7" s="29">
+        <v>999</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="29">
+        <f t="shared" si="0"/>
+        <v>502</v>
+      </c>
+      <c r="L7" s="29">
+        <f>F7</f>
+        <v>502</v>
+      </c>
+      <c r="M7" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="26">
+        <v>5</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="29">
+        <v>501</v>
+      </c>
+      <c r="F8" s="29">
+        <v>505</v>
+      </c>
+      <c r="G8" s="29">
+        <v>0</v>
+      </c>
+      <c r="H8" s="29">
+        <v>101</v>
+      </c>
+      <c r="I8" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="K8" s="29">
+        <f t="shared" si="0"/>
+        <v>505</v>
+      </c>
+      <c r="L8" s="29">
+        <f t="shared" ref="L8:L11" si="1">F8</f>
+        <v>505</v>
+      </c>
+      <c r="M8" s="29">
+        <f>K8/H8</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="26">
+        <v>6</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="D9" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="29">
+        <v>501</v>
+      </c>
+      <c r="F9" s="29">
+        <v>666</v>
+      </c>
+      <c r="G9" s="29">
+        <v>0</v>
+      </c>
+      <c r="H9" s="29">
+        <v>60</v>
+      </c>
+      <c r="I9" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" s="29">
+        <f t="shared" si="0"/>
+        <v>666</v>
+      </c>
+      <c r="L9" s="29">
+        <f t="shared" si="1"/>
+        <v>666</v>
+      </c>
+      <c r="M9" s="29">
+        <f t="shared" ref="M9:M11" si="2">K9/H9</f>
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="26">
+        <v>7</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="29">
+        <v>501</v>
+      </c>
+      <c r="F10" s="29">
+        <v>666</v>
+      </c>
+      <c r="G10" s="29">
+        <v>0</v>
+      </c>
+      <c r="H10" s="29">
+        <v>120</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="29">
+        <f t="shared" si="0"/>
+        <v>666</v>
+      </c>
+      <c r="L10" s="29">
+        <f t="shared" si="1"/>
+        <v>666</v>
+      </c>
+      <c r="M10" s="29">
+        <f t="shared" si="2"/>
+        <v>5.55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="26">
+        <v>8</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="29">
+        <v>501</v>
+      </c>
+      <c r="F11" s="29">
+        <v>666</v>
+      </c>
+      <c r="G11" s="29">
+        <v>0</v>
+      </c>
+      <c r="H11" s="29">
+        <v>180</v>
+      </c>
+      <c r="I11" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" s="29">
+        <f t="shared" si="0"/>
+        <v>666</v>
+      </c>
+      <c r="L11" s="29">
+        <f t="shared" si="1"/>
+        <v>666</v>
+      </c>
+      <c r="M11" s="29">
+        <f t="shared" si="2"/>
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>177</v>
+      </c>
+      <c r="B16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C16" t="s">
+        <v>179</v>
+      </c>
+      <c r="D16" t="s">
+        <v>180</v>
+      </c>
+      <c r="E16" t="s">
+        <v>181</v>
+      </c>
+      <c r="F16" t="s">
+        <v>182</v>
+      </c>
+      <c r="G16" t="s">
+        <v>183</v>
+      </c>
+      <c r="H16" t="s">
+        <v>184</v>
+      </c>
+      <c r="I16" t="s">
+        <v>185</v>
+      </c>
+      <c r="J16" t="s">
+        <v>186</v>
+      </c>
+      <c r="K16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" t="s">
+        <v>46</v>
+      </c>
+      <c r="K17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="F19" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="G19" t="s">
+        <v>46</v>
+      </c>
+      <c r="H19" t="s">
+        <v>46</v>
+      </c>
+      <c r="I19" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" t="s">
+        <v>46</v>
+      </c>
+      <c r="K19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C20" t="s">
+        <v>109</v>
+      </c>
+      <c r="D20" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="F20" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="G20" s="76" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="76" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="76" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="K20" s="30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="E21" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="G21" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="I21" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="J21" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="K21" s="30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="F22" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="G22" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="H22" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="I22" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="J22" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="K22" s="30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="78" t="s">
+        <v>109</v>
+      </c>
+      <c r="E23" s="78" t="s">
+        <v>110</v>
+      </c>
+      <c r="F23" s="78" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="H23" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="I23" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="J23" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="K23" s="30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="78" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" s="78" t="s">
+        <v>110</v>
+      </c>
+      <c r="F24" s="78" t="s">
+        <v>109</v>
+      </c>
+      <c r="G24" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="H24" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="I24" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="J24" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="K24" s="30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
+      <c r="B31" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11">
+      <c r="D32" t="s">
+        <v>180</v>
+      </c>
+      <c r="E32" t="s">
+        <v>181</v>
+      </c>
+      <c r="F32" t="s">
+        <v>182</v>
+      </c>
+      <c r="G32" t="s">
+        <v>187</v>
+      </c>
+      <c r="H32" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9">
+      <c r="B33" t="s">
+        <v>190</v>
+      </c>
+      <c r="D33" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="F33" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="G33" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="H33">
+        <v>501</v>
+      </c>
+      <c r="I33" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9">
+      <c r="B34" t="s">
+        <v>188</v>
+      </c>
+      <c r="D34" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="E34" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="F34" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="G34" s="77" t="s">
+        <v>109</v>
+      </c>
+      <c r="H34">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9">
+      <c r="B35" t="s">
+        <v>189</v>
+      </c>
+      <c r="D35" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="E35" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="F35" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="G35" s="77" t="s">
+        <v>109</v>
+      </c>
+      <c r="H35">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9">
+      <c r="B36" t="s">
+        <v>191</v>
+      </c>
+      <c r="D36" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="E36" s="75" t="s">
+        <v>110</v>
+      </c>
+      <c r="F36" s="75" t="s">
+        <v>109</v>
+      </c>
+      <c r="G36" s="77" t="s">
+        <v>109</v>
+      </c>
+      <c r="H36">
+        <v>666</v>
+      </c>
+      <c r="I36" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9">
+      <c r="B39" t="s">
+        <v>198</v>
+      </c>
+      <c r="D39" t="s">
+        <v>183</v>
+      </c>
+      <c r="E39" t="s">
+        <v>184</v>
+      </c>
+      <c r="F39" t="s">
+        <v>185</v>
+      </c>
+      <c r="G39" t="s">
+        <v>186</v>
+      </c>
+      <c r="H39" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9">
+      <c r="B40">
+        <v>999</v>
+      </c>
+      <c r="D40" s="76" t="s">
+        <v>46</v>
+      </c>
+      <c r="E40" s="76" t="s">
+        <v>46</v>
+      </c>
+      <c r="F40" s="76" t="s">
+        <v>46</v>
+      </c>
+      <c r="G40" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="H40" s="77" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9">
+      <c r="B41">
+        <v>179</v>
+      </c>
+      <c r="D41" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="E41" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="F41" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="G41" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="H41" s="77" t="s">
+        <v>109</v>
+      </c>
+      <c r="I41" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9">
+      <c r="B42">
+        <v>60</v>
+      </c>
+      <c r="D42" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="E42" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="F42" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="G42" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="H42" s="77" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9">
+      <c r="B43">
+        <v>120</v>
+      </c>
+      <c r="D43" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="E43" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="F43" s="76" t="s">
+        <v>109</v>
+      </c>
+      <c r="G43" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="H43" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="I43" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9">
+      <c r="B44">
+        <v>180</v>
+      </c>
+      <c r="D44" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="E44" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="F44" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="G44" s="76" t="s">
+        <v>110</v>
+      </c>
+      <c r="H44" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="I44" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:H1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:M2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>